<commit_message>
correction: ahora se puede calificar el examen al estudiante
</commit_message>
<xml_diff>
--- a/resources/usuarios.xlsx
+++ b/resources/usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\G\mesas-examen\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765ABAA3-7D48-43D5-9890-240240451B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F28F3D-5690-4B2B-854E-7ADA022DF9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D3B38E61-6CEB-4F52-98DD-F3030B71C668}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3B38E61-6CEB-4F52-98DD-F3030B71C668}"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes" sheetId="1" r:id="rId1"/>
@@ -7067,12 +7067,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA4F1BD-F148-4823-A9DD-605DA8CF9BE1}">
   <dimension ref="A1:I661"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26254,10 +26255,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E96396-EC00-4D11-A7AB-0F668C40D868}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>